<commit_message>
Fix: change boiling plan weights
</commit_message>
<xml_diff>
--- a/app/data/static/params/ricotta.xlsx
+++ b/app/data/static/params/ricotta.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="95">
   <si>
     <t xml:space="preserve">Название SKU</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Перекачивание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Внесение ингредиентов</t>
   </si>
   <si>
     <t xml:space="preserve">Kод</t>
@@ -311,7 +314,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -347,12 +350,6 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -418,10 +415,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,16 +435,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -511,8 +501,11 @@
       <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,19 +513,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>50</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>0.25</v>
@@ -573,8 +566,11 @@
       <c r="T2" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>23</v>
+      <c r="U2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,19 +578,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>0.5</v>
@@ -635,8 +631,11 @@
       <c r="T3" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U3" s="3" t="s">
-        <v>25</v>
+      <c r="U3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,19 +643,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="3" t="n">
         <v>0.2</v>
@@ -697,8 +696,11 @@
       <c r="T4" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>28</v>
+      <c r="U4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,19 +708,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>0.5</v>
@@ -759,8 +761,11 @@
       <c r="T5" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U5" s="3" t="s">
-        <v>31</v>
+      <c r="U5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,19 +773,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="3" t="n">
         <v>0.2</v>
@@ -821,8 +826,11 @@
       <c r="T6" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>33</v>
+      <c r="U6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,19 +838,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>0.2</v>
@@ -883,8 +891,11 @@
       <c r="T7" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U7" s="3" t="s">
-        <v>36</v>
+      <c r="U7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,22 +903,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H8" s="3" t="n">
         <v>0.2</v>
@@ -948,8 +959,11 @@
       <c r="T8" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>40</v>
+      <c r="U8" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,22 +971,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H9" s="3" t="n">
         <v>0.2</v>
@@ -1013,8 +1027,11 @@
       <c r="T9" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>43</v>
+      <c r="U9" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,22 +1039,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H10" s="3" t="n">
         <v>0.2</v>
@@ -1078,8 +1095,11 @@
       <c r="T10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>46</v>
+      <c r="U10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,22 +1107,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>0.2</v>
@@ -1143,8 +1163,11 @@
       <c r="T11" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U11" s="3" t="s">
-        <v>49</v>
+      <c r="U11" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,22 +1175,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" s="3" t="n">
         <v>0.2</v>
@@ -1208,8 +1231,11 @@
       <c r="T12" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U12" s="3" t="s">
-        <v>51</v>
+      <c r="U12" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,22 +1243,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H13" s="3" t="n">
         <v>0.2</v>
@@ -1273,8 +1299,11 @@
       <c r="T13" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U13" s="3" t="s">
-        <v>54</v>
+      <c r="U13" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,19 +1311,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H14" s="3" t="n">
         <v>0.5</v>
@@ -1335,8 +1364,11 @@
       <c r="T14" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U14" s="3" t="s">
-        <v>57</v>
+      <c r="U14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,22 +1376,22 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H15" s="3" t="n">
         <v>0.2</v>
@@ -1400,8 +1432,11 @@
       <c r="T15" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U15" s="3" t="s">
-        <v>59</v>
+      <c r="U15" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,22 +1444,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>0.2</v>
@@ -1465,8 +1500,11 @@
       <c r="T16" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U16" s="3" t="s">
-        <v>62</v>
+      <c r="U16" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,19 +1512,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3" t="n">
         <v>0.25</v>
@@ -1527,8 +1565,11 @@
       <c r="T17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U17" s="3" t="s">
-        <v>64</v>
+      <c r="U17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,19 +1577,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H18" s="3" t="n">
         <v>0.2</v>
@@ -1589,8 +1630,11 @@
       <c r="T18" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U18" s="3" t="s">
-        <v>67</v>
+      <c r="U18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,19 +1642,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H19" s="3" t="n">
         <v>0.2</v>
@@ -1651,8 +1695,11 @@
       <c r="T19" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U19" s="3" t="s">
-        <v>70</v>
+      <c r="U19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,22 +1707,22 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H20" s="3" t="n">
         <v>0.2</v>
@@ -1716,8 +1763,11 @@
       <c r="T20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U20" s="3" t="s">
-        <v>72</v>
+      <c r="U20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,19 +1775,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H21" s="3" t="n">
         <v>0.2</v>
@@ -1778,8 +1828,11 @@
       <c r="T21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U21" s="3" t="s">
-        <v>74</v>
+      <c r="U21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,22 +1840,22 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H22" s="3" t="n">
         <v>0.2</v>
@@ -1843,8 +1896,11 @@
       <c r="T22" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U22" s="3" t="s">
-        <v>76</v>
+      <c r="U22" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,22 +1908,22 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H23" s="3" t="n">
         <v>0.18</v>
@@ -1881,7 +1937,7 @@
       <c r="K23" s="3" t="n">
         <v>700</v>
       </c>
-      <c r="L23" s="4" t="n">
+      <c r="L23" s="3" t="n">
         <v>350</v>
       </c>
       <c r="M23" s="3" t="n">
@@ -1908,8 +1964,11 @@
       <c r="T23" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U23" s="3" t="s">
-        <v>78</v>
+      <c r="U23" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,22 +1976,22 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H24" s="3" t="n">
         <v>0.14</v>
@@ -1946,7 +2005,7 @@
       <c r="K24" s="3" t="n">
         <v>700</v>
       </c>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="3" t="n">
         <v>350</v>
       </c>
       <c r="M24" s="3" t="n">
@@ -1973,8 +2032,11 @@
       <c r="T24" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U24" s="3" t="s">
-        <v>80</v>
+      <c r="U24" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,19 +2044,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>25</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H25" s="3" t="n">
         <v>0.5</v>
@@ -2008,7 +2070,7 @@
       <c r="K25" s="3" t="n">
         <v>700</v>
       </c>
-      <c r="L25" s="4" t="n">
+      <c r="L25" s="3" t="n">
         <v>350</v>
       </c>
       <c r="M25" s="3" t="n">
@@ -2035,8 +2097,11 @@
       <c r="T25" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U25" s="3" t="s">
-        <v>82</v>
+      <c r="U25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,19 +2109,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>50</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3" t="n">
         <v>0.2</v>
@@ -2097,8 +2162,11 @@
       <c r="T26" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U26" s="3" t="s">
-        <v>84</v>
+      <c r="U26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,19 +2174,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H27" s="3" t="n">
         <v>2.5</v>
@@ -2159,8 +2227,11 @@
       <c r="T27" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U27" s="3" t="s">
-        <v>86</v>
+      <c r="U27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,19 +2239,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>45</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H28" s="3" t="n">
         <v>0.2</v>
@@ -2221,8 +2292,11 @@
       <c r="T28" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U28" s="3" t="s">
-        <v>89</v>
+      <c r="U28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,22 +2304,22 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>30</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H29" s="3" t="n">
         <v>0.2</v>
@@ -2286,8 +2360,11 @@
       <c r="T29" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U29" s="3" t="s">
-        <v>91</v>
+      <c r="U29" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2295,19 +2372,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>25</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H30" s="3" t="n">
         <v>1.4</v>
@@ -2348,8 +2425,11 @@
       <c r="T30" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U30" s="3" t="s">
-        <v>93</v>
+      <c r="U30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>